<commit_message>
refactor: atualização das screenshots com dados aleatorios
</commit_message>
<xml_diff>
--- a/ProjetoCusto_MaquinasPesadas.xlsx
+++ b/ProjetoCusto_MaquinasPesadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\diego.b.silva\Desktop\Projeto_MaquinasPesadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BEB7D2-FCA9-45F6-A2EC-6B1B6BED8F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D9A154-BCC9-4DCC-B8C3-1CCD2DBAE1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-2280" windowWidth="24240" windowHeight="13020" xr2:uid="{F400FFF7-B425-4B0C-9418-4E9096806235}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F400FFF7-B425-4B0C-9418-4E9096806235}"/>
   </bookViews>
   <sheets>
     <sheet name="Custo Manutenção" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -303,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -328,69 +327,22 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -398,10 +350,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -409,10 +379,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -427,77 +430,133 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -862,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FEBC2B-8B1F-4E4F-BD2F-F63E68735D5C}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -888,152 +947,196 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A2" s="3">
         <v>45658</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="2">
+      <c r="C2" s="20">
+        <f ca="1">RANDBETWEEN(1000,45000)</f>
+        <v>29350</v>
+      </c>
+      <c r="D2" s="23">
+        <f ca="1">RANDBETWEEN(5000,30000)</f>
+        <v>28260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A3" s="4">
         <v>45689</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="2">
+      <c r="C3" s="21">
+        <f t="shared" ref="C3:C13" ca="1" si="0">RANDBETWEEN(1000,45000)</f>
+        <v>39347</v>
+      </c>
+      <c r="D3" s="24">
+        <f t="shared" ref="D3:D13" ca="1" si="1">RANDBETWEEN(5000,30000)</f>
+        <v>13891</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A4" s="4">
         <v>45717</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A5" s="2">
+      <c r="C4" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>37199</v>
+      </c>
+      <c r="D4" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>11460</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A5" s="4">
         <v>45748</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="2">
+      <c r="C5" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>20805</v>
+      </c>
+      <c r="D5" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>28221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A6" s="4">
         <v>45778</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="2">
+      <c r="C6" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>22952</v>
+      </c>
+      <c r="D6" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>24995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A7" s="4">
         <v>45809</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10">
-        <v>41012.200000000004</v>
-      </c>
-      <c r="D7" s="10">
-        <v>29213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A8" s="2">
+      <c r="C7" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>25706</v>
+      </c>
+      <c r="D7" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>18820</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A8" s="4">
         <v>45839</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10">
-        <v>11444.73</v>
-      </c>
-      <c r="D8" s="10">
-        <v>10443.709999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A9" s="2">
+      <c r="C8" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>8901</v>
+      </c>
+      <c r="D8" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>14209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A9" s="4">
         <v>45870</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10">
-        <v>21678.15</v>
-      </c>
-      <c r="D9" s="10">
-        <v>4406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="2">
+      <c r="C9" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>21639</v>
+      </c>
+      <c r="D9" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>19284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A10" s="4">
         <v>45901</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="10">
-        <v>48182.87</v>
-      </c>
-      <c r="D10" s="10">
-        <v>8688</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A11" s="2">
+      <c r="C10" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>2987</v>
+      </c>
+      <c r="D10" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>11019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A11" s="4">
         <v>45931</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="10">
-        <v>29283.83</v>
-      </c>
-      <c r="D11" s="10">
-        <v>12121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A12" s="2">
+      <c r="C11" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>39853</v>
+      </c>
+      <c r="D11" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>20631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A12" s="4">
         <v>45962</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10">
-        <v>20275.23</v>
-      </c>
-      <c r="D12" s="10">
-        <v>26680</v>
+      <c r="C12" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>30341</v>
+      </c>
+      <c r="D12" s="24">
+        <f t="shared" ca="1" si="1"/>
+        <v>8649</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A13" s="2">
+      <c r="A13" s="5">
         <v>45992</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="10">
-        <v>18236.169999999998</v>
-      </c>
-      <c r="D13" s="10">
-        <v>2805</v>
+      <c r="C13" s="22">
+        <f t="shared" ca="1" si="0"/>
+        <v>12728</v>
+      </c>
+      <c r="D13" s="25">
+        <f t="shared" ca="1" si="1"/>
+        <v>20463</v>
       </c>
     </row>
   </sheetData>
@@ -1047,7 +1150,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="C2" activeCellId="3" sqref="A2:A13 B2:B13 C1 C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,160 +1168,204 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="2">
+    <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A2" s="3">
         <v>45658</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="2">
+      <c r="C2" s="14">
+        <f ca="1">RANDBETWEEN(1500,10000)</f>
+        <v>5472</v>
+      </c>
+      <c r="D2" s="9">
+        <f ca="1">RANDBETWEEN(15000,50000)</f>
+        <v>20721</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A3" s="4">
         <v>45689</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="2">
+      <c r="C3" s="15">
+        <f t="shared" ref="C3:C13" ca="1" si="0">RANDBETWEEN(1500,10000)</f>
+        <v>8136</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" ref="D3:D13" ca="1" si="1">RANDBETWEEN(15000,50000)</f>
+        <v>38418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A4" s="4">
         <v>45717</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A5" s="2">
+      <c r="C4" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>8367</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>30539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A5" s="4">
         <v>45748</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="2">
+      <c r="C5" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>2975</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>44192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A6" s="4">
         <v>45778</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="2">
+      <c r="C6" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>9855</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>26194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A7" s="4">
         <v>45809</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="20">
-        <v>1958.6</v>
+      <c r="C7" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>2916</v>
       </c>
       <c r="D7" s="10">
-        <v>11326.36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>42382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A8" s="4">
         <v>45839</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20">
-        <v>4455.8</v>
+      <c r="C8" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>6921</v>
       </c>
       <c r="D8" s="10">
-        <v>26200.09</v>
-      </c>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>37582</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A9" s="4">
         <v>45870</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="20">
-        <v>4187.5</v>
+      <c r="C9" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1796</v>
       </c>
       <c r="D9" s="10">
-        <v>24990.859999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>42194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A10" s="4">
         <v>45901</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="20">
-        <v>3525.5</v>
+      <c r="C10" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>4992</v>
       </c>
       <c r="D10" s="10">
-        <v>21258.73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A11" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47945</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A11" s="4">
         <v>45931</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="20">
-        <v>4075.3</v>
+      <c r="C11" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1720</v>
       </c>
       <c r="D11" s="10">
-        <v>24696.27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A12" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>48160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A12" s="4">
         <v>45962</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="20">
-        <v>4024.6</v>
+      <c r="C12" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>9167</v>
       </c>
       <c r="D12" s="10">
-        <v>24590.3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>34637</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A13" s="2">
+      <c r="A13" s="5">
         <v>45992</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="20">
-        <v>4975.5</v>
-      </c>
-      <c r="D13" s="10">
-        <v>30748.560000000001</v>
+      <c r="C13" s="16">
+        <f t="shared" ca="1" si="0"/>
+        <v>5497</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" ca="1" si="1"/>
+        <v>40273</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1379,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1277,258 +1424,402 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="2">
+    <row r="2" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A2" s="3">
         <v>45658</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="26">
         <v>0.95</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="2">
+      <c r="D2" s="29">
+        <f ca="1">RANDBETWEEN(75,100)/100</f>
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="29">
+        <f t="shared" ref="E2:I2" ca="1" si="0">RANDBETWEEN(75,100)/100</f>
+        <v>0.76</v>
+      </c>
+      <c r="F2" s="29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="G2" s="29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.84</v>
+      </c>
+      <c r="H2" s="29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A3" s="4">
         <v>45689</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="2">
+      <c r="C3" s="27"/>
+      <c r="D3" s="30">
+        <f t="shared" ref="D3:I13" ca="1" si="1">RANDBETWEEN(75,100)/100</f>
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83</v>
+      </c>
+      <c r="F3" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="G3" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H3" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99</v>
+      </c>
+      <c r="I3" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A4" s="4">
         <v>45717</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A5" s="2">
+      <c r="C4" s="27"/>
+      <c r="D4" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77</v>
+      </c>
+      <c r="E4" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="F4" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91</v>
+      </c>
+      <c r="G4" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.94</v>
+      </c>
+      <c r="H4" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="I4" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A5" s="4">
         <v>45748</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="2">
+      <c r="C5" s="27"/>
+      <c r="D5" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99</v>
+      </c>
+      <c r="E5" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.96</v>
+      </c>
+      <c r="G5" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A6" s="4">
         <v>45778</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="2">
+      <c r="C6" s="27"/>
+      <c r="D6" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.78</v>
+      </c>
+      <c r="E6" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="F6" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.89</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A7" s="4">
         <v>45809</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A8" s="2">
+      <c r="C7" s="27"/>
+      <c r="D7" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.94</v>
+      </c>
+      <c r="F7" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.98</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A8" s="4">
         <v>45839</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="6">
-        <v>0.98</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="C8" s="27"/>
+      <c r="D8" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.82</v>
+      </c>
+      <c r="E8" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="F8" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99</v>
+      </c>
+      <c r="H8" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A9" s="4">
+        <v>45870</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="H9" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A10" s="4">
+        <v>45901</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93</v>
+      </c>
+      <c r="E10" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88</v>
+      </c>
+      <c r="F10" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.89</v>
+      </c>
+      <c r="G10" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.81</v>
+      </c>
+      <c r="H10" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.76</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A11" s="4">
+        <v>45931</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.96</v>
+      </c>
+      <c r="E11" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="F11" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.94</v>
+      </c>
+      <c r="G11" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="H11" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" ca="1" si="1"/>
         <v>0.92</v>
       </c>
-      <c r="F8" s="6">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A9" s="2">
-        <v>45870</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="6">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="2">
-        <v>45901</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="6">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.95</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A11" s="2">
-        <v>45931</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="6">
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0.872</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A12" s="2">
+    </row>
+    <row r="12" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.7">
+      <c r="A12" s="4">
         <v>45962</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="6">
-        <v>0.96660000000000001</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.87770000000000004</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0.71109999999999995</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0.98880000000000001</v>
-      </c>
-      <c r="H12" s="6">
+      <c r="C12" s="27"/>
+      <c r="D12" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85</v>
+      </c>
+      <c r="E12" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79</v>
+      </c>
+      <c r="F12" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77</v>
+      </c>
+      <c r="G12" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.78</v>
+      </c>
+      <c r="H12" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A13" s="5">
+        <v>45992</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85</v>
+      </c>
+      <c r="E13" s="31">
+        <f t="shared" ca="1" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="I12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A13" s="2">
-        <v>45992</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0.86899999999999999</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1</v>
+      <c r="F13" s="31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93</v>
+      </c>
+      <c r="G13" s="31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="H13" s="31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="I13" s="31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88</v>
       </c>
     </row>
   </sheetData>
@@ -1554,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9A7279-9ADF-4390-8CED-BF1B83B5F0A2}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,7 +1859,7 @@
     <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.4" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1589,176 +1880,211 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="16">
-        <v>339890</v>
-      </c>
-      <c r="F2" s="16"/>
+      <c r="E2" s="36">
+        <v>455000</v>
+      </c>
+      <c r="F2" s="36">
+        <f ca="1">RANDBETWEEN(50000,120000)</f>
+        <v>105635</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="E3" s="37">
+        <v>350000</v>
+      </c>
+      <c r="F3" s="37">
+        <f t="shared" ref="F3:F11" ca="1" si="0">RANDBETWEEN(50000,120000)</f>
+        <v>82135</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="E4" s="37">
+        <v>22000</v>
+      </c>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="37">
+        <v>240000</v>
+      </c>
+      <c r="F5" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>86649</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="16">
-        <v>120000</v>
-      </c>
-      <c r="F6" s="16"/>
+      <c r="E6" s="37">
+        <v>250000</v>
+      </c>
+      <c r="F6" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>69810</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="37">
+        <v>236000</v>
+      </c>
+      <c r="F7" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>89155</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="16">
-        <v>470000</v>
-      </c>
-      <c r="F8" s="16"/>
+      <c r="E8" s="37">
+        <v>540000</v>
+      </c>
+      <c r="F8" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>80077</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="16">
-        <v>550000</v>
-      </c>
-      <c r="F9" s="16"/>
+      <c r="E9" s="37">
+        <v>500000</v>
+      </c>
+      <c r="F9" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>100347</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="16">
-        <v>550000</v>
-      </c>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.7">
-      <c r="A11" s="15" t="s">
+      <c r="E10" s="37">
+        <v>650000</v>
+      </c>
+      <c r="F10" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>67573</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A11" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="16">
-        <v>910800</v>
-      </c>
-      <c r="F11" s="16"/>
+      <c r="E11" s="38">
+        <v>1135000</v>
+      </c>
+      <c r="F11" s="38">
+        <f t="shared" ca="1" si="0"/>
+        <v>69766</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>